<commit_message>
Convites sem espaços v2.
</commit_message>
<xml_diff>
--- a/Convites Encontrão ECC.xlsx
+++ b/Convites Encontrão ECC.xlsx
@@ -15,13 +15,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -60,15 +65,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
+      <xdr:colOff>438150</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -86,7 +91,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="47625" y="47625"/>
+          <a:off x="0" y="0"/>
           <a:ext cx="2876550" cy="2162175"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -105,62 +110,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1026" name="Imagem 22"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3200400" y="57150"/>
-          <a:ext cx="2876550" cy="2162175"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -178,7 +137,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="47625" y="2219325"/>
+          <a:off x="0" y="2171700"/>
           <a:ext cx="2876550" cy="2162175"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -198,15 +157,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
+      <xdr:colOff>438150</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -224,7 +183,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="47625" y="6562725"/>
+          <a:off x="0" y="6505575"/>
           <a:ext cx="2876550" cy="2162175"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -243,154 +202,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1030" name="Imagem 27"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3200400" y="2228850"/>
-          <a:ext cx="2876550" cy="2152650"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1031" name="Imagem 28"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3200400" y="4400550"/>
-          <a:ext cx="2876550" cy="2152650"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1032" name="Imagem 29"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3200400" y="6562725"/>
-          <a:ext cx="2876550" cy="2152650"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
+      <xdr:colOff>438150</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -408,7 +229,191 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="47625" y="4400550"/>
+          <a:off x="0" y="4343400"/>
+          <a:ext cx="2876550" cy="2152650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1041" name="Imagem 21"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2886075" y="0"/>
+          <a:ext cx="2876550" cy="2162175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1042" name="Imagem 23"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2886075" y="2171700"/>
+          <a:ext cx="2876550" cy="2162175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1043" name="Imagem 25"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2886075" y="6505575"/>
+          <a:ext cx="2876550" cy="2162175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1044" name="Imagem 24"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2886075" y="4343400"/>
           <a:ext cx="2876550" cy="2152650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -693,13 +698,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <phoneticPr fontId="0" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.59055118110236227" right="0.31496062992125984" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>